<commit_message>
Wokring in My Points
</commit_message>
<xml_diff>
--- a/public/files/Upload_Order_Sample_File.xlsx
+++ b/public/files/Upload_Order_Sample_File.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>StateDate</t>
-  </si>
-  <si>
     <t>EndDate</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>FullDescriptionHindi</t>
+  </si>
+  <si>
+    <t>StartDate</t>
   </si>
 </sst>
 </file>
@@ -314,7 +314,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -333,22 +333,22 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>

</xml_diff>